<commit_message>
HU aumento de gestión y seguimiento de silabo
HU aumento de gestión y seguimiento de silabo
</commit_message>
<xml_diff>
--- a/HU_GestiónÁreaCarrera_01.xlsx
+++ b/HU_GestiónÁreaCarrera_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ALCI\Documents\GitHub\UniversidadDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CE37B0-20CB-495D-8AAF-232A281A32EC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40299CC7-BC9F-4F77-8E68-35E2E872B058}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="76">
   <si>
     <t>HISTORIAS DE USUARIO</t>
   </si>
@@ -200,13 +200,61 @@
   </si>
   <si>
     <t>UN-CAR-017</t>
+  </si>
+  <si>
+    <t>UN-CAR-18</t>
+  </si>
+  <si>
+    <t>Necesito gestionar sílabos</t>
+  </si>
+  <si>
+    <t>Con la finalidad de gestionar la temática a tratarse en cada materia y las características del mismo</t>
+  </si>
+  <si>
+    <t>UN-CAR-19</t>
+  </si>
+  <si>
+    <t>Necesito gestionar temas</t>
+  </si>
+  <si>
+    <t>Con la finalidad de determinar los temas a tratarse en la asignatura (Parciales)</t>
+  </si>
+  <si>
+    <t>UN-CAR-20</t>
+  </si>
+  <si>
+    <t>Necesito gestionar subtemas</t>
+  </si>
+  <si>
+    <t>Con la finalidad de determinar los subtemas asignados a cada parcial.</t>
+  </si>
+  <si>
+    <t>UN-CAR-21</t>
+  </si>
+  <si>
+    <t>Necesito gestionar tareas</t>
+  </si>
+  <si>
+    <t>Con la finalidad de definir las tareas a ser resueltas por los estudiantes a lo largo del semestre y a qué subtema pertenecen.</t>
+  </si>
+  <si>
+    <t>UN-CAR-22</t>
+  </si>
+  <si>
+    <t>Como estudiante</t>
+  </si>
+  <si>
+    <t>Necesito realizar el seguimiento al sílabo</t>
+  </si>
+  <si>
+    <t>Con la finalidad de validar los subtemas que ya han sido dados en clase.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -230,8 +278,20 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,8 +322,20 @@
         <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -349,11 +421,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -383,6 +470,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -727,11 +823,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:E51"/>
+  <dimension ref="B2:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50:B51"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1189,45 +1286,218 @@
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
     </row>
+    <row r="52" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B52" s="13"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+    </row>
+    <row r="53" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+    </row>
+    <row r="55" spans="2:5" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B55" s="14"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+    </row>
+    <row r="56" spans="2:5" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="14"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+    </row>
+    <row r="57" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="15"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+    </row>
+    <row r="58" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B58" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E58" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B59" s="14"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+    </row>
+    <row r="60" spans="2:5" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B60" s="14"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+    </row>
+    <row r="61" spans="2:5" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="14"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+    </row>
+    <row r="62" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B62" s="15"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="15"/>
+    </row>
+    <row r="63" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B63" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E63" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B64" s="14"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14"/>
+    </row>
+    <row r="65" spans="2:5" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B65" s="14"/>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+    </row>
+    <row r="66" spans="2:5" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B66" s="14"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+    </row>
+    <row r="67" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B67" s="15"/>
+      <c r="C67" s="15"/>
+      <c r="D67" s="15"/>
+      <c r="E67" s="15"/>
+    </row>
+    <row r="68" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B68" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D68" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E68" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B69" s="14"/>
+      <c r="C69" s="14"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="14"/>
+    </row>
+    <row r="70" spans="2:5" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B70" s="14"/>
+      <c r="C70" s="14"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="14"/>
+    </row>
+    <row r="71" spans="2:5" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="14"/>
+      <c r="C71" s="14"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="14"/>
+    </row>
+    <row r="72" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B72" s="15"/>
+      <c r="C72" s="15"/>
+      <c r="D72" s="15"/>
+      <c r="E72" s="15"/>
+    </row>
+    <row r="73" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B73" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C73" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D73" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E73" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B74" s="14"/>
+      <c r="C74" s="14"/>
+      <c r="D74" s="14"/>
+      <c r="E74" s="14"/>
+    </row>
+    <row r="75" spans="2:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B75" s="14"/>
+      <c r="C75" s="14"/>
+      <c r="D75" s="14"/>
+      <c r="E75" s="14"/>
+    </row>
+    <row r="76" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B76" s="15"/>
+      <c r="C76" s="15"/>
+      <c r="D76" s="15"/>
+      <c r="E76" s="15"/>
+    </row>
   </sheetData>
-  <mergeCells count="61">
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="E22:E23"/>
+  <mergeCells count="81">
+    <mergeCell ref="B73:B75"/>
+    <mergeCell ref="C73:C75"/>
+    <mergeCell ref="D73:D75"/>
+    <mergeCell ref="E73:E75"/>
+    <mergeCell ref="B53:B56"/>
+    <mergeCell ref="C53:C56"/>
+    <mergeCell ref="D53:D56"/>
+    <mergeCell ref="E53:E56"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="C58:C61"/>
+    <mergeCell ref="D58:D61"/>
+    <mergeCell ref="E58:E61"/>
+    <mergeCell ref="B63:B66"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="D63:D66"/>
+    <mergeCell ref="E63:E66"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="C68:C71"/>
+    <mergeCell ref="D68:D71"/>
+    <mergeCell ref="E68:E71"/>
     <mergeCell ref="B50:B51"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="D31:D32"/>
@@ -1238,21 +1508,59 @@
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E44:E45"/>
     <mergeCell ref="B47:B48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="D25:D26"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="D38:D39"/>
     <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="D25:D26"/>
     <mergeCell ref="E38:E39"/>
-    <mergeCell ref="B41:B42"/>
     <mergeCell ref="E41:E42"/>
     <mergeCell ref="E25:E26"/>
-    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B22:B23"/>
     <mergeCell ref="B28:B29"/>
     <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B7:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="81" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>